<commit_message>
Adición del IMT con una prueba para el clasificador
</commit_message>
<xml_diff>
--- a/IMT/IMT.xlsx
+++ b/IMT/IMT.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\home\chrisbermudezr\Indices_Climaticos\IMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD9DA9D-7562-464B-A1FC-638AE35BDFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3387CB5E-829F-4F98-8725-F4790BEB9615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-70" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-70" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indices" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indices!$A$1:$W$774</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indices!$A$1:$J$774</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6194" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6324" uniqueCount="39">
   <si>
     <t>date</t>
   </si>
@@ -506,19 +507,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J774"/>
+  <dimension ref="A1:J779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35:I35"/>
+    <sheetView topLeftCell="E745" workbookViewId="0">
+      <selection activeCell="A770" sqref="A770:J779"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" customWidth="1"/>
+    <col min="4" max="4" width="255.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
     <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
@@ -25139,7 +25140,7 @@
         <v>45658</v>
       </c>
       <c r="B770">
-        <v>0.7</v>
+        <v>0.49569999999999997</v>
       </c>
       <c r="C770" t="s">
         <v>8</v>
@@ -25171,7 +25172,7 @@
         <v>45689</v>
       </c>
       <c r="B771">
-        <v>1.5</v>
+        <v>0.84289999999999998</v>
       </c>
       <c r="C771" t="s">
         <v>8</v>
@@ -25183,16 +25184,16 @@
         <v>10</v>
       </c>
       <c r="F771" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G771" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H771" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I771" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J771" t="s">
         <v>13</v>
@@ -25203,7 +25204,7 @@
         <v>45717</v>
       </c>
       <c r="B772">
-        <v>1.9</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="C772" t="s">
         <v>8</v>
@@ -25215,16 +25216,16 @@
         <v>10</v>
       </c>
       <c r="F772" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G772" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H772" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I772" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J772" t="s">
         <v>13</v>
@@ -25235,7 +25236,7 @@
         <v>45748</v>
       </c>
       <c r="B773">
-        <v>1.6</v>
+        <v>0.3332</v>
       </c>
       <c r="C773" t="s">
         <v>8</v>
@@ -25247,16 +25248,16 @@
         <v>10</v>
       </c>
       <c r="F773" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G773" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H773" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I773" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J773" t="s">
         <v>13</v>
@@ -25267,7 +25268,7 @@
         <v>45778</v>
       </c>
       <c r="B774">
-        <v>1.2</v>
+        <v>0.30359999999999998</v>
       </c>
       <c r="C774" t="s">
         <v>8</v>
@@ -25279,23 +25280,563 @@
         <v>10</v>
       </c>
       <c r="F774" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G774" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H774" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I774" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J774" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="775" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A775" s="2">
+        <v>45809</v>
+      </c>
+      <c r="B775">
+        <v>0.90759999999999996</v>
+      </c>
+      <c r="C775" t="s">
+        <v>8</v>
+      </c>
+      <c r="D775" t="s">
+        <v>9</v>
+      </c>
+      <c r="E775" t="s">
+        <v>10</v>
+      </c>
+      <c r="F775" t="s">
+        <v>14</v>
+      </c>
+      <c r="G775" t="s">
+        <v>15</v>
+      </c>
+      <c r="H775" t="s">
+        <v>33</v>
+      </c>
+      <c r="I775" t="s">
+        <v>34</v>
+      </c>
+      <c r="J775" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="776" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A776" s="2">
+        <v>45839</v>
+      </c>
+      <c r="B776">
+        <v>0.8921</v>
+      </c>
+      <c r="C776" t="s">
+        <v>8</v>
+      </c>
+      <c r="D776" t="s">
+        <v>9</v>
+      </c>
+      <c r="E776" t="s">
+        <v>10</v>
+      </c>
+      <c r="F776" t="s">
+        <v>14</v>
+      </c>
+      <c r="G776" t="s">
+        <v>15</v>
+      </c>
+      <c r="H776" t="s">
+        <v>33</v>
+      </c>
+      <c r="I776" t="s">
+        <v>34</v>
+      </c>
+      <c r="J776" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="777" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A777" s="2">
+        <v>45870</v>
+      </c>
+      <c r="B777">
+        <v>0.5212</v>
+      </c>
+      <c r="C777" t="s">
+        <v>8</v>
+      </c>
+      <c r="D777" t="s">
+        <v>9</v>
+      </c>
+      <c r="E777" t="s">
+        <v>10</v>
+      </c>
+      <c r="F777" t="s">
+        <v>14</v>
+      </c>
+      <c r="G777" t="s">
+        <v>15</v>
+      </c>
+      <c r="H777" t="s">
+        <v>33</v>
+      </c>
+      <c r="I777" t="s">
+        <v>34</v>
+      </c>
+      <c r="J777" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="778" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A778" s="2">
+        <v>45901</v>
+      </c>
+      <c r="B778">
+        <v>-1.3357000000000001</v>
+      </c>
+      <c r="C778" t="s">
+        <v>8</v>
+      </c>
+      <c r="D778" t="s">
+        <v>9</v>
+      </c>
+      <c r="E778" t="s">
+        <v>10</v>
+      </c>
+      <c r="F778" t="s">
+        <v>16</v>
+      </c>
+      <c r="G778" t="s">
+        <v>17</v>
+      </c>
+      <c r="H778" t="s">
+        <v>29</v>
+      </c>
+      <c r="I778" t="s">
+        <v>36</v>
+      </c>
+      <c r="J778" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="779" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A779" s="2">
+        <v>45931</v>
+      </c>
+      <c r="B779">
+        <v>-1.5083</v>
+      </c>
+      <c r="C779" t="s">
+        <v>8</v>
+      </c>
+      <c r="D779" t="s">
+        <v>9</v>
+      </c>
+      <c r="E779" t="s">
+        <v>10</v>
+      </c>
+      <c r="F779" t="s">
+        <v>16</v>
+      </c>
+      <c r="G779" t="s">
+        <v>17</v>
+      </c>
+      <c r="H779" t="s">
+        <v>29</v>
+      </c>
+      <c r="I779" t="s">
+        <v>36</v>
+      </c>
+      <c r="J779" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:W774" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J774" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93A028A-6F58-4708-9C50-6A161987D1D3}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>45658</v>
+      </c>
+      <c r="B2">
+        <v>0.49569999999999997</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>45689</v>
+      </c>
+      <c r="B3">
+        <v>0.84289999999999998</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>45717</v>
+      </c>
+      <c r="B4">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>45748</v>
+      </c>
+      <c r="B5">
+        <v>0.3332</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>45778</v>
+      </c>
+      <c r="B6">
+        <v>0.30359999999999998</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>45809</v>
+      </c>
+      <c r="B7">
+        <v>0.90759999999999996</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>45839</v>
+      </c>
+      <c r="B8">
+        <v>0.8921</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>45870</v>
+      </c>
+      <c r="B9">
+        <v>0.5212</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>45901</v>
+      </c>
+      <c r="B10">
+        <v>-1.3357000000000001</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>45931</v>
+      </c>
+      <c r="B11">
+        <v>-1.5083</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>